<commit_message>
Sortino Ratio Part Update
</commit_message>
<xml_diff>
--- a/Portfolio Optimisation/annual_returns.xlsx
+++ b/Portfolio Optimisation/annual_returns.xlsx
@@ -8,17 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ergodique/Documents/GitHub/Portfolio/Portfolio Optimisation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DF4ADD-4839-DD48-AA8D-FB054A27F44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9B64F4-E3D6-2D4D-9B7A-7FAD3E144A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33240" yWindow="2260" windowWidth="27640" windowHeight="16020" activeTab="5" xr2:uid="{19ED1665-9CBF-DD4E-BAD7-EBE5CB4B4DE0}"/>
+    <workbookView xWindow="33240" yWindow="2260" windowWidth="27640" windowHeight="16020" activeTab="4" xr2:uid="{19ED1665-9CBF-DD4E-BAD7-EBE5CB4B4DE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet8" sheetId="9" r:id="rId2"/>
+    <sheet name="Sheet9" sheetId="10" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet10" sheetId="11" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId7"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId8"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId9"/>
+    <sheet name="Sheet7" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="7">
   <si>
     <t>TCD</t>
   </si>
@@ -59,12 +63,15 @@
   <si>
     <t>VIOP30</t>
   </si>
+  <si>
+    <t>AHI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,6 +113,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -127,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -136,6 +151,7 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,221 +466,257 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C5A738-1BD5-9A4A-B608-6E222E4265E2}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G9"/>
+      <selection sqref="A1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>2023</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="7">
+        <v>-13.757999999999999</v>
+      </c>
+      <c r="C2" s="2">
         <v>-16.957999999999998</v>
       </c>
-      <c r="C2" s="7">
+      <c r="D2" s="7">
         <v>-22.015000000000001</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>3.5289999999999999</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>7.9969999999999999</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>68.27</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>-13.458020000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2022</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="7">
+        <v>269.798</v>
+      </c>
+      <c r="C3" s="2">
         <v>220.429</v>
       </c>
-      <c r="C3" s="7">
+      <c r="D3" s="7">
         <v>286.79500000000002</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>46.32</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>-0.33100000000000002</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>-81.02</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>198.73989499999999</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2021</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="7">
+        <v>43.564</v>
+      </c>
+      <c r="C4" s="2">
         <v>34.993000000000002</v>
       </c>
-      <c r="C4" s="7">
+      <c r="D4" s="7">
         <v>27.17</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>78.391000000000005</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>-3.746</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>90</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>27.146312000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2020</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="7">
+        <v>46.259</v>
+      </c>
+      <c r="C5" s="2">
         <v>115.32599999999999</v>
       </c>
-      <c r="C5" s="7">
+      <c r="D5" s="7">
         <v>94.4</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>32.140999999999998</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>25.231000000000002</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>301</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>17.159554</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>2019</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="7">
+        <v>33.786999999999999</v>
+      </c>
+      <c r="C6" s="2">
         <v>127.36499999999999</v>
       </c>
-      <c r="C6" s="7">
+      <c r="D6" s="7">
         <v>74.05</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>27.866</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>18.367999999999999</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>95</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>19.944775</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>2018</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="7">
+        <v>-15.632</v>
+      </c>
+      <c r="C7" s="2">
         <v>3.319</v>
       </c>
-      <c r="C7" s="7">
+      <c r="D7" s="7">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>32.454000000000001</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>-1.6020000000000001</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>-73</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>-19.217570000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>2017</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="7">
+        <v>32.478000000000002</v>
+      </c>
+      <c r="C8" s="2">
         <v>12.840999999999999</v>
       </c>
-      <c r="C8" s="7">
+      <c r="D8" s="7">
         <v>20.228000000000002</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>16.678999999999998</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>13.21</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>1331</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>51.415951999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>2016</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="7">
+        <v>8.2050000000000001</v>
+      </c>
+      <c r="C9" s="2">
         <v>10.818</v>
       </c>
-      <c r="C9" s="7">
+      <c r="D9" s="7">
         <v>20.405000000000001</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>10.125</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>-10.622999999999999</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>125</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>8.7288139999999999</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="7"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -672,6 +724,173 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE77DFF9-6C8F-ED47-9F8D-21626B9D26A7}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B2" s="7">
+        <v>-13.757999999999999</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-16.957999999999998</v>
+      </c>
+      <c r="D2" s="7">
+        <v>-22.015000000000001</v>
+      </c>
+      <c r="E2" s="1">
+        <v>7.9969999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B3" s="7">
+        <v>269.798</v>
+      </c>
+      <c r="C3" s="2">
+        <v>220.429</v>
+      </c>
+      <c r="D3" s="7">
+        <v>286.79500000000002</v>
+      </c>
+      <c r="E3" s="1">
+        <v>-0.33100000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B4" s="7">
+        <v>43.564</v>
+      </c>
+      <c r="C4" s="2">
+        <v>34.993000000000002</v>
+      </c>
+      <c r="D4" s="7">
+        <v>27.17</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-3.746</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B5" s="7">
+        <v>46.259</v>
+      </c>
+      <c r="C5" s="2">
+        <v>115.32599999999999</v>
+      </c>
+      <c r="D5" s="7">
+        <v>94.4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>25.231000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B6" s="7">
+        <v>33.786999999999999</v>
+      </c>
+      <c r="C6" s="2">
+        <v>127.36499999999999</v>
+      </c>
+      <c r="D6" s="7">
+        <v>74.05</v>
+      </c>
+      <c r="E6" s="1">
+        <v>18.367999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B7" s="7">
+        <v>-15.632</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3.319</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-1.6020000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>2017</v>
+      </c>
+      <c r="B8" s="7">
+        <v>32.478000000000002</v>
+      </c>
+      <c r="C8" s="2">
+        <v>12.840999999999999</v>
+      </c>
+      <c r="D8" s="7">
+        <v>20.228000000000002</v>
+      </c>
+      <c r="E8" s="1">
+        <v>13.21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>2016</v>
+      </c>
+      <c r="B9" s="7">
+        <v>8.2050000000000001</v>
+      </c>
+      <c r="C9" s="2">
+        <v>10.818</v>
+      </c>
+      <c r="D9" s="7">
+        <v>20.405000000000001</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-10.622999999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -679,6 +898,311 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2E7CEE2-9471-BD4F-8415-26D8A2AF24DE}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3.5289999999999999</v>
+      </c>
+      <c r="C2" s="2">
+        <v>68.27</v>
+      </c>
+      <c r="D2" s="2">
+        <v>-13.458019999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>2022</v>
+      </c>
+      <c r="B3" s="2">
+        <v>46.32</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-81.02</v>
+      </c>
+      <c r="D3" s="2">
+        <v>198.73989499999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B4" s="2">
+        <v>78.391000000000005</v>
+      </c>
+      <c r="C4" s="2">
+        <v>90</v>
+      </c>
+      <c r="D4" s="2">
+        <v>27.146312000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B5" s="2">
+        <v>32.140999999999998</v>
+      </c>
+      <c r="C5" s="2">
+        <v>301</v>
+      </c>
+      <c r="D5" s="2">
+        <v>17.159554</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B6" s="2">
+        <v>27.866</v>
+      </c>
+      <c r="C6" s="2">
+        <v>95</v>
+      </c>
+      <c r="D6" s="2">
+        <v>19.944775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>2018</v>
+      </c>
+      <c r="B7" s="2">
+        <v>32.454000000000001</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-73</v>
+      </c>
+      <c r="D7" s="2">
+        <v>-19.217569999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>2017</v>
+      </c>
+      <c r="B8" s="2">
+        <v>16.678999999999998</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1331</v>
+      </c>
+      <c r="D8" s="2">
+        <v>51.415951999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>2016</v>
+      </c>
+      <c r="B9" s="2">
+        <v>10.125</v>
+      </c>
+      <c r="C9" s="2">
+        <v>125</v>
+      </c>
+      <c r="D9" s="2">
+        <v>8.7288139999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94FB4A34-7EFB-2348-AA93-6CC5008164F4}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3.5289999999999999</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-13.458019999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>2022</v>
+      </c>
+      <c r="B3" s="2">
+        <v>46.32</v>
+      </c>
+      <c r="C3" s="2">
+        <v>198.73989499999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B4" s="2">
+        <v>78.391000000000005</v>
+      </c>
+      <c r="C4" s="2">
+        <v>27.146312000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B5" s="2">
+        <v>32.140999999999998</v>
+      </c>
+      <c r="C5" s="2">
+        <v>17.159554</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B6" s="2">
+        <v>27.866</v>
+      </c>
+      <c r="C6" s="2">
+        <v>19.944775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>2018</v>
+      </c>
+      <c r="B7" s="2">
+        <v>32.454000000000001</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-19.217569999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>2017</v>
+      </c>
+      <c r="B8" s="2">
+        <v>16.678999999999998</v>
+      </c>
+      <c r="C8" s="2">
+        <v>51.415951999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>2016</v>
+      </c>
+      <c r="B9" s="2">
+        <v>10.125</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8.7288139999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE653C2B-277A-234E-893E-6AB66419B616}">
   <dimension ref="A1:D31"/>
   <sheetViews>
@@ -904,7 +1428,164 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72BB08F3-F97F-074A-A900-59267F4A6359}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>2023</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-16.957999999999998</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3.5289999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>2022</v>
+      </c>
+      <c r="B3" s="2">
+        <v>220.429</v>
+      </c>
+      <c r="C3" s="2">
+        <v>46.32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>2021</v>
+      </c>
+      <c r="B4" s="2">
+        <v>34.993000000000002</v>
+      </c>
+      <c r="C4" s="2">
+        <v>78.391000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>2020</v>
+      </c>
+      <c r="B5" s="2">
+        <v>115.32599999999999</v>
+      </c>
+      <c r="C5" s="2">
+        <v>32.140999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>2019</v>
+      </c>
+      <c r="B6" s="2">
+        <v>127.36499999999999</v>
+      </c>
+      <c r="C6" s="2">
+        <v>27.866</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>2018</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3.319</v>
+      </c>
+      <c r="C7" s="2">
+        <v>32.454000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>2017</v>
+      </c>
+      <c r="B8" s="2">
+        <v>12.840999999999999</v>
+      </c>
+      <c r="C8" s="2">
+        <v>16.678999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>2016</v>
+      </c>
+      <c r="B9" s="2">
+        <v>10.818</v>
+      </c>
+      <c r="C9" s="2">
+        <v>10.125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{024D41E7-6164-754F-8294-D191DEA13CAC}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -1016,7 +1697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6574C986-8C2F-B743-90B9-CA7741C295BC}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -1137,7 +1818,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{135BC247-7E84-3843-A0A7-B8FB6FF61A03}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -1276,11 +1957,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089E4465-244D-894A-B1AC-D75600CFD5A2}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
monte carlo and portfolio optimisation last trys
</commit_message>
<xml_diff>
--- a/Portfolio Optimisation/annual_returns.xlsx
+++ b/Portfolio Optimisation/annual_returns.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Icons\Git Repos\Erdo Portfolio\Portfolio\Portfolio Optimisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4379EF5-A8D5-494A-834E-84CA1FE7FF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE71FD7-C190-493E-88EE-F107F9E28495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{19ED1665-9CBF-DD4E-BAD7-EBE5CB4B4DE0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{19ED1665-9CBF-DD4E-BAD7-EBE5CB4B4DE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="16" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="17" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="18" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t>BTC</t>
   </si>
@@ -57,7 +58,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -105,10 +106,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1400,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C5AF81-174B-419D-8049-E36CC0E976E0}">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2193,4 +2194,635 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D2AD48-AFFB-4811-89FD-3B5F04F266E8}">
+  <dimension ref="A1:C56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>43831</v>
+      </c>
+      <c r="B2">
+        <v>4.68</v>
+      </c>
+      <c r="C2">
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>43862</v>
+      </c>
+      <c r="B3">
+        <v>1.24</v>
+      </c>
+      <c r="C3">
+        <v>0.10299999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>43891</v>
+      </c>
+      <c r="B4">
+        <v>3.82</v>
+      </c>
+      <c r="C4">
+        <v>-7.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>43922</v>
+      </c>
+      <c r="B5">
+        <v>13.69</v>
+      </c>
+      <c r="C5">
+        <v>1.292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>43952</v>
+      </c>
+      <c r="B6">
+        <v>8.0909999999999993</v>
+      </c>
+      <c r="C6">
+        <v>-1.0720000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>43983</v>
+      </c>
+      <c r="B7">
+        <v>10.228</v>
+      </c>
+      <c r="C7">
+        <v>0.36099999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>44013</v>
+      </c>
+      <c r="B8">
+        <v>-3.2850000000000001</v>
+      </c>
+      <c r="C8">
+        <v>3.3170000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>44044</v>
+      </c>
+      <c r="B9">
+        <v>-2.7090000000000001</v>
+      </c>
+      <c r="C9">
+        <v>3.4620000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>44075</v>
+      </c>
+      <c r="B10">
+        <v>4.7590000000000003</v>
+      </c>
+      <c r="C10">
+        <v>11.193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>44105</v>
+      </c>
+      <c r="B11">
+        <v>1.4510000000000001</v>
+      </c>
+      <c r="C11">
+        <v>8.3829999999999991</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>44136</v>
+      </c>
+      <c r="B12">
+        <v>13.269</v>
+      </c>
+      <c r="C12">
+        <v>1.8859999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>44166</v>
+      </c>
+      <c r="B13">
+        <v>20.661999999999999</v>
+      </c>
+      <c r="C13">
+        <v>7.0190000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>44197</v>
+      </c>
+      <c r="B14">
+        <v>4.5380000000000003</v>
+      </c>
+      <c r="C14">
+        <v>4.8520000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>44228</v>
+      </c>
+      <c r="B15">
+        <v>1.58</v>
+      </c>
+      <c r="C15">
+        <v>3.859</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>44256</v>
+      </c>
+      <c r="B16">
+        <v>-2.448</v>
+      </c>
+      <c r="C16">
+        <v>1.8260000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>44287</v>
+      </c>
+      <c r="B17">
+        <v>2.1259999999999999</v>
+      </c>
+      <c r="C17">
+        <v>1.5109999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>44317</v>
+      </c>
+      <c r="B18">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="C18">
+        <v>6.3339999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>44348</v>
+      </c>
+      <c r="B19">
+        <v>-5.4429999999999996</v>
+      </c>
+      <c r="C19">
+        <v>-1.4530000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>44378</v>
+      </c>
+      <c r="B20">
+        <v>3.923</v>
+      </c>
+      <c r="C20">
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>44409</v>
+      </c>
+      <c r="B21">
+        <v>5.6340000000000003</v>
+      </c>
+      <c r="C21">
+        <v>1.0189999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>44440</v>
+      </c>
+      <c r="B22">
+        <v>-3.5409999999999999</v>
+      </c>
+      <c r="C22">
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>44470</v>
+      </c>
+      <c r="B23">
+        <v>7.7610000000000001</v>
+      </c>
+      <c r="C23">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>44501</v>
+      </c>
+      <c r="B24">
+        <v>16.68</v>
+      </c>
+      <c r="C24">
+        <v>19.061</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>44531</v>
+      </c>
+      <c r="B25">
+        <v>3.8780000000000001</v>
+      </c>
+      <c r="C25">
+        <v>-8.4909999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>44562</v>
+      </c>
+      <c r="B26">
+        <v>9.4079999999999995</v>
+      </c>
+      <c r="C26">
+        <v>7.0839999999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>44593</v>
+      </c>
+      <c r="B27">
+        <v>-4.383</v>
+      </c>
+      <c r="C27">
+        <v>-7.3010000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>44621</v>
+      </c>
+      <c r="B28">
+        <v>14.97</v>
+      </c>
+      <c r="C28">
+        <v>14.288</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>44652</v>
+      </c>
+      <c r="B29">
+        <v>12.061</v>
+      </c>
+      <c r="C29">
+        <v>12.872999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>44682</v>
+      </c>
+      <c r="B30">
+        <v>3.202</v>
+      </c>
+      <c r="C30">
+        <v>4.3529999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>44713</v>
+      </c>
+      <c r="B31">
+        <v>-3.802</v>
+      </c>
+      <c r="C31">
+        <v>-0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>44743</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>8.4160000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>44774</v>
+      </c>
+      <c r="B33">
+        <v>24.41</v>
+      </c>
+      <c r="C33">
+        <v>16.190999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>44805</v>
+      </c>
+      <c r="B34">
+        <v>0.745</v>
+      </c>
+      <c r="C34">
+        <v>9.3140000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>44835</v>
+      </c>
+      <c r="B35">
+        <v>24.411999999999999</v>
+      </c>
+      <c r="C35">
+        <v>18.811</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>44866</v>
+      </c>
+      <c r="B36">
+        <v>26.701000000000001</v>
+      </c>
+      <c r="C36">
+        <v>23.09</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>44896</v>
+      </c>
+      <c r="B37">
+        <v>12.461</v>
+      </c>
+      <c r="C37">
+        <v>16.106999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>44927</v>
+      </c>
+      <c r="B38">
+        <v>-9.6270000000000007</v>
+      </c>
+      <c r="C38">
+        <v>-9.4749999999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>44958</v>
+      </c>
+      <c r="B39">
+        <v>1.3360000000000001</v>
+      </c>
+      <c r="C39">
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>44986</v>
+      </c>
+      <c r="B40">
+        <v>-1.4910000000000001</v>
+      </c>
+      <c r="C40">
+        <v>4.1120000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>45017</v>
+      </c>
+      <c r="B41">
+        <v>2.8290000000000002</v>
+      </c>
+      <c r="C41">
+        <v>4.8710000000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>45047</v>
+      </c>
+      <c r="B42">
+        <v>4.8310000000000004</v>
+      </c>
+      <c r="C42">
+        <v>7.7679999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>45078</v>
+      </c>
+      <c r="B43">
+        <v>23.010999999999999</v>
+      </c>
+      <c r="C43">
+        <v>23.794</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>45108</v>
+      </c>
+      <c r="B44">
+        <v>28.763999999999999</v>
+      </c>
+      <c r="C44">
+        <v>23.853999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>45139</v>
+      </c>
+      <c r="B45">
+        <v>22.725000000000001</v>
+      </c>
+      <c r="C45">
+        <v>4.6070000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>45170</v>
+      </c>
+      <c r="B46">
+        <v>8.5589999999999993</v>
+      </c>
+      <c r="C46">
+        <v>14.397</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>45200</v>
+      </c>
+      <c r="B47">
+        <v>-5.1749999999999998</v>
+      </c>
+      <c r="C47">
+        <v>-1.9410000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>45231</v>
+      </c>
+      <c r="B48">
+        <v>6.2389999999999999</v>
+      </c>
+      <c r="C48">
+        <v>11.045</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>45261</v>
+      </c>
+      <c r="B49">
+        <v>-1.3160000000000001</v>
+      </c>
+      <c r="C49">
+        <v>-0.378</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>45292</v>
+      </c>
+      <c r="B50">
+        <v>14.401</v>
+      </c>
+      <c r="C50">
+        <v>4.9160000000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>45323</v>
+      </c>
+      <c r="B51">
+        <v>6.4359999999999999</v>
+      </c>
+      <c r="C51">
+        <v>10.709</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>45352</v>
+      </c>
+      <c r="B52">
+        <v>4.266</v>
+      </c>
+      <c r="C52">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>45383</v>
+      </c>
+      <c r="B53">
+        <v>16.942</v>
+      </c>
+      <c r="C53">
+        <v>7.3550000000000004</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>45413</v>
+      </c>
+      <c r="B54">
+        <v>8.7799999999999994</v>
+      </c>
+      <c r="C54">
+        <v>4.1269999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>45444</v>
+      </c>
+      <c r="B55">
+        <v>7.0549999999999997</v>
+      </c>
+      <c r="C55">
+        <v>5.2549999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>45474</v>
+      </c>
+      <c r="B56">
+        <v>0.127</v>
+      </c>
+      <c r="C56">
+        <v>7.5590000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
some fixes and ticker selection part for portfolio optimization
</commit_message>
<xml_diff>
--- a/Portfolio Optimisation/annual_returns.xlsx
+++ b/Portfolio Optimisation/annual_returns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Icons\Git Repos\Erdo Portfolio\Portfolio\Portfolio Optimisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE71FD7-C190-493E-88EE-F107F9E28495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A98698-1BC1-4BD7-8285-D363F08FD6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{19ED1665-9CBF-DD4E-BAD7-EBE5CB4B4DE0}"/>
+    <workbookView xWindow="31530" yWindow="3705" windowWidth="21600" windowHeight="11505" activeTab="2" xr2:uid="{19ED1665-9CBF-DD4E-BAD7-EBE5CB4B4DE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="16" r:id="rId1"/>
@@ -426,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9F2E0B-0218-4B41-AA2E-5DB018F5BF60}">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection sqref="A1:E56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1399,10 +1399,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C5AF81-174B-419D-8049-E36CC0E976E0}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2191,6 +2191,34 @@
         <v>7.5590000000000002</v>
       </c>
     </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>45505</v>
+      </c>
+      <c r="B57">
+        <v>-1.637</v>
+      </c>
+      <c r="C57">
+        <v>-5.4189999999999996</v>
+      </c>
+      <c r="D57">
+        <v>4.7439999999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>45536</v>
+      </c>
+      <c r="B58">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="C58">
+        <v>2.403</v>
+      </c>
+      <c r="D58">
+        <v>1.641</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2198,10 +2226,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D2AD48-AFFB-4811-89FD-3B5F04F266E8}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2822,6 +2850,28 @@
         <v>7.5590000000000002</v>
       </c>
     </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>45505</v>
+      </c>
+      <c r="B57">
+        <v>-5.4189999999999996</v>
+      </c>
+      <c r="C57">
+        <v>4.7439999999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>45536</v>
+      </c>
+      <c r="B58">
+        <v>2.403</v>
+      </c>
+      <c r="C58">
+        <v>1.641</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>